<commit_message>
Customizing XForms (translations and extra variables)
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/DEATHTOHOH.xlsx
+++ b/xforms/xlsforms/DEATHTOHOH.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="285" windowWidth="21600" windowHeight="9840" tabRatio="500"/>
+    <workbookView xWindow="630" yWindow="1890" windowWidth="21600" windowHeight="9840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="173">
   <si>
     <t>type</t>
   </si>
@@ -189,12 +189,6 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Death to Head of household</t>
-  </si>
-  <si>
     <t>membershiptonewhoh</t>
   </si>
   <si>
@@ -406,13 +400,148 @@
   </si>
   <si>
     <t>concat(${causeofdeathdiagnosed},${causofdeathnotdiagnosed})</t>
+  </si>
+  <si>
+    <t>label::Portuguese</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Morte do chefe do agregado</t>
+  </si>
+  <si>
+    <t>concat("DDTHOH-",${permId})</t>
+  </si>
+  <si>
+    <t>permId</t>
+  </si>
+  <si>
+    <t>Perm ID</t>
+  </si>
+  <si>
+    <t>Id da visita</t>
+  </si>
+  <si>
+    <t>ExtId do Individuo</t>
+  </si>
+  <si>
+    <t>Novo ID do Chefe de agregado</t>
+  </si>
+  <si>
+    <t>Código do Inquiridor</t>
+  </si>
+  <si>
+    <t>Id do Agregado</t>
+  </si>
+  <si>
+    <t>Causa da morte</t>
+  </si>
+  <si>
+    <t>As causas da morte foram diagnósticadas pelas autoridades de saúde?</t>
+  </si>
+  <si>
+    <t>Quem diagnosticou?</t>
+  </si>
+  <si>
+    <t>Causa da morte diagnosticadas?</t>
+  </si>
+  <si>
+    <t>Causa da morte não diagnosticadas?</t>
+  </si>
+  <si>
+    <t>Local da morte</t>
+  </si>
+  <si>
+    <t>Introduza o Local da morte</t>
+  </si>
+  <si>
+    <t>Resultados</t>
+  </si>
+  <si>
+    <t>Relação com o chefe de agregado</t>
+  </si>
+  <si>
+    <t>Nova Filiação</t>
+  </si>
+  <si>
+    <t>ExtId do Membro</t>
+  </si>
+  <si>
+    <t>Nome do membro</t>
+  </si>
+  <si>
+    <t>Filho/a</t>
+  </si>
+  <si>
+    <t>Irmã/o</t>
+  </si>
+  <si>
+    <t>Sem relação</t>
+  </si>
+  <si>
+    <t>Outra relação</t>
+  </si>
+  <si>
+    <t>Não sabe</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Médico</t>
+  </si>
+  <si>
+    <t>Enfermeira</t>
+  </si>
+  <si>
+    <t>Trabalhador comunitario de saude</t>
+  </si>
+  <si>
+    <t>Médico Tradicional</t>
+  </si>
+  <si>
+    <t>Tuberculose</t>
+  </si>
+  <si>
+    <t>Outro tipo de infecção</t>
+  </si>
+  <si>
+    <t>Acidente</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>Doença</t>
+  </si>
+  <si>
+    <t>Clinica ou Centro médico</t>
+  </si>
+  <si>
+    <t>Neto/a</t>
+  </si>
+  <si>
+    <t>Em Casa</t>
+  </si>
+  <si>
+    <t>Data da morte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1603,41 +1732,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="30.125" style="5" customWidth="1"/>
     <col min="2" max="2" width="26.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="37.25" style="5" customWidth="1"/>
-    <col min="4" max="4" width="30.125" style="5" customWidth="1"/>
+    <col min="3" max="4" width="30.125" style="5" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="5" customWidth="1"/>
     <col min="6" max="6" width="22.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="25" style="5" customWidth="1"/>
-    <col min="8" max="9" width="10.875" style="5"/>
-    <col min="10" max="10" width="19.125" style="5" customWidth="1"/>
-    <col min="11" max="15" width="10.875" style="5"/>
-    <col min="16" max="16" width="12" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="5"/>
+    <col min="8" max="8" width="10.875" style="5"/>
+    <col min="9" max="9" width="37.25" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.875" style="5"/>
+    <col min="11" max="11" width="19.125" style="5" customWidth="1"/>
+    <col min="12" max="16" width="10.875" style="5"/>
+    <col min="17" max="17" width="12" style="5" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>7</v>
+      <c r="C1" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>17</v>
@@ -1654,32 +1784,35 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -1694,13 +1827,14 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -1715,13 +1849,14 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1736,141 +1871,160 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H6" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>66</v>
+        <v>133</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="L7" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>64</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="H8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L8" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>124</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="H9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K9" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L9" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="36">
+      <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="C12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1878,20 +2032,20 @@
       <c r="H12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1899,20 +2053,23 @@
       <c r="H13" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1920,236 +2077,294 @@
       <c r="H14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="H16" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="C17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="H17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:17" ht="36">
+      <c r="A18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="K18" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K17" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="L18" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="13.5" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="5" t="b">
+      <c r="B19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="L19" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="24">
+      <c r="A20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="Q20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>68</v>
+        <v>58</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>150</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="H21" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K21" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="L21" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>23</v>
+        <v>66</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="H22" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K22" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>42</v>
+      <c r="L22" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="H23" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="D24" s="9"/>
+      <c r="L23" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="24.75" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="H24" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="K25" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H26" s="3"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L26" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="H27" s="3"/>
+    </row>
+    <row r="35" spans="8:8">
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="8:8">
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="8:8">
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="8:8">
       <c r="H38" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="8:8">
+      <c r="H39" s="3"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
+    <row r="60" spans="1:8">
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
+      <c r="A63" s="3"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H65" s="3"/>
+    <row r="64" spans="1:8">
+      <c r="H64" s="3"/>
+    </row>
+    <row r="66" spans="8:8">
+      <c r="H66" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2158,515 +2373,619 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.25" style="12" customWidth="1"/>
-    <col min="2" max="2" width="18.625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.75" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="12"/>
+    <col min="2" max="2" width="29.625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="27.125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="18.75" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="15">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="15">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="15">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="15">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="15">
         <v>5</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="15">
         <v>6</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="15">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="15">
         <v>2</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="21" customFormat="1">
       <c r="A10" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>95</v>
+      <c r="C10" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="21" customFormat="1">
       <c r="A11" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>96</v>
+      <c r="C11" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="21" customFormat="1">
       <c r="A12" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B12" s="15">
         <v>3</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>97</v>
+      <c r="C12" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="21" customFormat="1">
       <c r="A13" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="15">
         <v>4</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="21" customFormat="1">
+      <c r="A14" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="D14" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="21" customFormat="1">
+      <c r="A15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E15" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="15" t="s">
+    <row r="16" spans="1:5" s="21" customFormat="1">
+      <c r="A16" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C16" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="21" customFormat="1">
+      <c r="A17" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="15" t="s">
+      <c r="C17" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="E17" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="15" t="s">
+    </row>
+    <row r="18" spans="1:5" s="21" customFormat="1">
+      <c r="A18" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C18" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="21" customFormat="1">
+      <c r="A19" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="C19" s="15" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="D19" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="21" customFormat="1">
+      <c r="A20" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C20" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="E20" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="15" t="s">
+    <row r="21" spans="1:5" s="21" customFormat="1">
+      <c r="A21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C21" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="E21" s="15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="15" t="s">
+    <row r="22" spans="1:5" s="21" customFormat="1">
+      <c r="A22" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C22" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="E22" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="15" t="s">
+    <row r="23" spans="1:5" s="21" customFormat="1">
+      <c r="A23" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="B23" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="21" customFormat="1">
+      <c r="A24" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="B24" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="21" customFormat="1">
+      <c r="A25" s="20" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>111</v>
-      </c>
       <c r="B25" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="21" customFormat="1">
+      <c r="A26" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C26" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="E26" s="15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="21" customFormat="1">
       <c r="A27" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="21" customFormat="1">
       <c r="A28" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="21" customFormat="1">
+      <c r="A29" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="C29" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="16" t="s">
+      <c r="E29" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="21" customFormat="1">
+      <c r="A30" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C30" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="16" t="s">
+    <row r="31" spans="1:5" s="21" customFormat="1">
+      <c r="A31" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C31" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E31" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="13"/>
       <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="13"/>
       <c r="B33" s="15"/>
-      <c r="C33" s="16"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="16"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="13"/>
       <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="16"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="13"/>
       <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="16"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="13"/>
       <c r="B36" s="15"/>
-      <c r="C36" s="16"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="16"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E36" s="16"/>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="13"/>
       <c r="B37" s="15"/>
-      <c r="C37" s="16"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="16"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E37" s="16"/>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="13"/>
       <c r="B38" s="15"/>
-      <c r="C38" s="16"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="16"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E38" s="16"/>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="13"/>
       <c r="B39" s="15"/>
-      <c r="C39" s="16"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="16"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="13"/>
       <c r="B40" s="15"/>
-      <c r="C40" s="16"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="16"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E40" s="16"/>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="13"/>
       <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
+      <c r="C41" s="15"/>
       <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2675,21 +2994,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="25.25" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -2699,16 +3019,22 @@
       <c r="C1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>